<commit_message>
Uploaded the updated presentation file
</commit_message>
<xml_diff>
--- a/QRcodesBurnDown-2.xlsx
+++ b/QRcodesBurnDown-2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Dropbox\QrCodesCSCI480\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reinhartm1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Down Chart Table" sheetId="1" r:id="rId1"/>
@@ -570,76 +570,76 @@
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>49</c:v>
+                  <c:v>35.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -763,11 +763,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="351193936"/>
-        <c:axId val="351195112"/>
+        <c:axId val="317032240"/>
+        <c:axId val="317031064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="351193936"/>
+        <c:axId val="317032240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,7 +872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351195112"/>
+        <c:crossAx val="317031064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -880,7 +880,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="351195112"/>
+        <c:axId val="317031064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,7 +1001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="351193936"/>
+        <c:crossAx val="317032240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1637,7 +1637,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1936,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2045,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="AC2" s="3">
         <f>(C2 - SUM(D2:AB2))</f>
-        <v>1</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="30" x14ac:dyDescent="0.25">
@@ -2133,7 +2133,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="AC3" s="3">
         <f>C3-(SUM(D3:AB3))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="30" x14ac:dyDescent="0.25">
@@ -2309,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="AC5" s="3">
         <f t="shared" ref="AC5:AC28" si="0">C5-(SUM(D5:AB5))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="30" x14ac:dyDescent="0.25">
@@ -2397,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
@@ -2473,7 +2473,7 @@
       </c>
       <c r="AC6" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="30" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="AC7" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="AC8" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="AC9" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
@@ -2758,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
         <v>0</v>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="AC10" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="AC11" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -3562,13 +3562,13 @@
         <v>0</v>
       </c>
       <c r="K19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="4">
         <v>0</v>
       </c>
       <c r="M19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="4">
         <v>0</v>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="AC19" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -3914,7 +3914,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="4">
         <v>0</v>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="AC23" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
@@ -4440,107 +4440,107 @@
       </c>
       <c r="D30" s="12">
         <f t="shared" ref="D30:AB30" si="1">C30-SUM(D2:D28)</f>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>38.5</v>
       </c>
       <c r="H30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>38.5</v>
       </c>
       <c r="I30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>38.5</v>
       </c>
       <c r="J30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>38.5</v>
       </c>
       <c r="K30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>36.5</v>
       </c>
       <c r="L30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>36.5</v>
       </c>
       <c r="M30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="N30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="O30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="P30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="Q30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="R30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="S30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="T30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="U30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="V30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="W30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="X30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="Y30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="Z30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="AA30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="AB30" s="12">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>35.5</v>
       </c>
       <c r="AC30" s="12">
         <f>SUM(AC2:AC28)</f>
-        <v>49</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Uploaded the corrected up to date Burn Down chart
</commit_message>
<xml_diff>
--- a/QRcodesBurnDown-2.xlsx
+++ b/QRcodesBurnDown-2.xlsx
@@ -570,76 +570,76 @@
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>39.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.5</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.5</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.5</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.5</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.5</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>35.5</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1936,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,7 +2045,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="AC2" s="3">
         <f>(C2 - SUM(D2:AB2))</f>
-        <v>-1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="30" x14ac:dyDescent="0.25">
@@ -2309,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="AC5" s="3">
         <f t="shared" ref="AC5:AC28" si="0">C5-(SUM(D5:AB5))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="30" x14ac:dyDescent="0.25">
@@ -2397,7 +2397,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
@@ -2473,7 +2473,7 @@
       </c>
       <c r="AC6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="30" x14ac:dyDescent="0.25">
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="AC8" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="45" x14ac:dyDescent="0.25">
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="AC9" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
@@ -2773,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="AC10" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="AC11" s="3">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="4">
         <v>0</v>
@@ -2937,7 +2937,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I12" s="4">
         <v>0</v>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="AC12" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
@@ -3128,7 +3128,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N14" s="4">
         <v>0</v>
@@ -3177,7 +3177,7 @@
       </c>
       <c r="AC14" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="45" x14ac:dyDescent="0.25">
@@ -3562,13 +3562,13 @@
         <v>0</v>
       </c>
       <c r="K19" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L19" s="4">
         <v>0</v>
       </c>
       <c r="M19" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N19" s="4">
         <v>0</v>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="AC19" s="3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -3653,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="L20" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="AC20" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
@@ -4440,107 +4440,107 @@
       </c>
       <c r="D30" s="12">
         <f t="shared" ref="D30:AB30" si="1">C30-SUM(D2:D28)</f>
-        <v>43</v>
+        <v>44.5</v>
       </c>
       <c r="E30" s="12">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>42.5</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>39.5</v>
       </c>
       <c r="G30" s="12">
         <f t="shared" si="1"/>
-        <v>38.5</v>
+        <v>36.5</v>
       </c>
       <c r="H30" s="12">
         <f t="shared" si="1"/>
-        <v>38.5</v>
+        <v>36</v>
       </c>
       <c r="I30" s="12">
         <f t="shared" si="1"/>
-        <v>38.5</v>
+        <v>36</v>
       </c>
       <c r="J30" s="12">
         <f t="shared" si="1"/>
-        <v>38.5</v>
+        <v>36</v>
       </c>
       <c r="K30" s="12">
         <f t="shared" si="1"/>
-        <v>36.5</v>
+        <v>34.5</v>
       </c>
       <c r="L30" s="12">
         <f t="shared" si="1"/>
-        <v>36.5</v>
+        <v>33</v>
       </c>
       <c r="M30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="N30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="O30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="P30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="Q30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="R30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="S30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="T30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="U30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="V30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="W30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="X30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="Y30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="Z30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="AA30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="AB30" s="12">
         <f t="shared" si="1"/>
-        <v>35.5</v>
+        <v>32</v>
       </c>
       <c r="AC30" s="12">
         <f>SUM(AC2:AC28)</f>
-        <v>35.5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>